<commit_message>
Bug fixes. Fixed the default regex, and the categorization scheme.
</commit_message>
<xml_diff>
--- a/output/NewsTest1.xlsx
+++ b/output/NewsTest1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Huwebes</t>
   </si>
@@ -39,9 +39,6 @@
     <t>NBI</t>
   </si>
   <si>
-    <t>Alex Diloy,</t>
-  </si>
-  <si>
     <t>PERSON</t>
   </si>
   <si>
@@ -106,6 +103,18 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Dacer at Corbito</t>
+  </si>
+  <si>
+    <t>Grace Amargo at Joy Cantos</t>
+  </si>
+  <si>
+    <t>Jimmy Lopez at Alex Diloy,</t>
+  </si>
+  <si>
+    <t>Lopez at Diloy</t>
   </si>
 </sst>
 </file>
@@ -916,7 +925,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,24 +966,24 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -988,175 +997,157 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D21" t="s">
         <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated result excel files.
</commit_message>
<xml_diff>
--- a/output/NewsTest1.xlsx
+++ b/output/NewsTest1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>Huwebes</t>
   </si>
@@ -115,6 +115,57 @@
   </si>
   <si>
     <t>Lopez at Diloy</t>
+  </si>
+  <si>
+    <t>Department of Justice</t>
+  </si>
+  <si>
+    <t>Gayunman,</t>
+  </si>
+  <si>
+    <t>Hiniling</t>
+  </si>
+  <si>
+    <t>Inaasahang,</t>
+  </si>
+  <si>
+    <t>Isinagawa ng DOJ</t>
+  </si>
+  <si>
+    <t>Isinagawa ng NBI</t>
+  </si>
+  <si>
+    <t>Ito</t>
+  </si>
+  <si>
+    <t>Kasabay</t>
+  </si>
+  <si>
+    <t>Nagbabala</t>
+  </si>
+  <si>
+    <t>National Bureau of Investigation</t>
+  </si>
+  <si>
+    <t>Nauna</t>
+  </si>
+  <si>
+    <t>PAOCTF</t>
+  </si>
+  <si>
+    <t>Pangulo</t>
+  </si>
+  <si>
+    <t>Presidential Anti-Organized Crime Task Force</t>
+  </si>
+  <si>
+    <t>Sa</t>
+  </si>
+  <si>
+    <t>Tukoy</t>
+  </si>
+  <si>
+    <t>Ulat</t>
   </si>
 </sst>
 </file>
@@ -922,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1056,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1016,7 +1067,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1027,7 +1078,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1038,7 +1089,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1049,7 +1100,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1060,7 +1111,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1071,7 +1122,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -1082,7 +1133,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1093,7 +1144,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -1104,7 +1155,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1115,7 +1166,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1126,7 +1177,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1136,18 +1187,148 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
       <c r="D19" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
       <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
       <c r="D21" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prioritizing person over location over date now when matching.
</commit_message>
<xml_diff>
--- a/output/NewsTest1.xlsx
+++ b/output/NewsTest1.xlsx
@@ -976,12 +976,13 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B35"/>
+      <selection activeCell="A5" sqref="A5:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
     <col min="4" max="4" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>